<commit_message>
Fixed unrecognized field bug
</commit_message>
<xml_diff>
--- a/Example/configuration_file.xlsx
+++ b/Example/configuration_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zacha\OneDrive\Desktop\Ualberta Summer 2022 Co-op\Processing_Folders\Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A1DA8E-A068-44BF-B3CE-EB6C1ECD561A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C523B31A-B1CA-4E44-B2C2-E1C0F39D95E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10940" yWindow="2713" windowWidth="13120" windowHeight="7660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="273" yWindow="2167" windowWidth="13120" windowHeight="7660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Mechanical Engineering</t>
   </si>
@@ -74,6 +74,12 @@
   </si>
   <si>
     <t>David S. Nobes</t>
+  </si>
+  <si>
+    <t>MecE 265</t>
+  </si>
+  <si>
+    <t>MecE 260</t>
   </si>
 </sst>
 </file>
@@ -394,7 +400,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -447,6 +453,12 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A4" t="s">

</xml_diff>

<commit_message>
Fixed bugs and transposed config file
</commit_message>
<xml_diff>
--- a/Example/configuration_file.xlsx
+++ b/Example/configuration_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zacha\OneDrive\Desktop\Ualberta Summer 2022 Co-op\Processing_Folders\Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C523B31A-B1CA-4E44-B2C2-E1C0F39D95E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D899A0-126D-4210-85A5-4D2E940D5D5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="273" yWindow="2167" windowWidth="13120" windowHeight="7660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Mechanical Engineering</t>
   </si>
@@ -80,6 +80,12 @@
   </si>
   <si>
     <t>MecE 260</t>
+  </si>
+  <si>
+    <t>Cagri Aryanci</t>
+  </si>
+  <si>
+    <t>MEC E 260</t>
   </si>
 </sst>
 </file>
@@ -400,13 +406,13 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="20.64453125" customWidth="1"/>
-    <col min="2" max="2" width="11.3515625" customWidth="1"/>
+    <col min="2" max="2" width="22.234375" customWidth="1"/>
     <col min="3" max="3" width="15.05859375" customWidth="1"/>
     <col min="4" max="4" width="17.3515625" customWidth="1"/>
     <col min="5" max="5" width="14.703125" customWidth="1"/>
@@ -417,60 +423,66 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>